<commit_message>
moved a lot into import script as to not have multiple lines in other scripts all doing the same thing
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustav Surface\Google Drive\DTU\02450 Introduktion til Machine Learning og Data Mining F20\02450Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3D9CFF-1743-44AD-BA96-3C9D65E9C41B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B568722-840F-4C81-A8A4-56ECE296875C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3003" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="744">
   <si>
     <t>doy</t>
   </si>
@@ -2247,6 +2247,21 @@
   </si>
   <si>
     <t>℉</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>ses</t>
+  </si>
+  <si>
+    <t>type2</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>A2</t>
   </si>
 </sst>
 </file>
@@ -2600,8 +2615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2654,6 +2669,9 @@
       <c r="K1" s="2" t="s">
         <v>724</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
@@ -2689,6 +2707,9 @@
       <c r="K2" t="s">
         <v>722</v>
       </c>
+      <c r="L2" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
@@ -2724,6 +2745,9 @@
       <c r="K3" t="s">
         <v>736</v>
       </c>
+      <c r="L3" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
@@ -2760,7 +2784,9 @@
         <f t="shared" ref="K4:K67" si="0">TEXT(DATE(1976,1,J4),"mmm")</f>
         <v>Jan</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
@@ -2797,7 +2823,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
@@ -2834,7 +2862,6 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" t="s">

</xml_diff>

<commit_message>
added option for classes being seasons rather than months
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustav Surface\Google Drive\DTU\02450 Introduktion til Machine Learning og Data Mining F20\02450Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B568722-840F-4C81-A8A4-56ECE296875C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09526B49-464B-4524-A8F6-2DC05252F0CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3336" uniqueCount="746">
   <si>
     <t>doy</t>
   </si>
@@ -2261,7 +2261,13 @@
     <t>Winter</t>
   </si>
   <si>
-    <t>A2</t>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Autumn</t>
   </si>
 </sst>
 </file>
@@ -2615,8 +2621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="D309" workbookViewId="0">
+      <selection activeCell="H316" sqref="H316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2785,7 +2791,7 @@
         <v>Jan</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.5">
@@ -2862,6 +2868,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
+      <c r="L6" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
@@ -2898,7 +2907,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
@@ -2935,7 +2946,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
@@ -2972,7 +2985,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
@@ -3009,7 +3024,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
@@ -3046,7 +3063,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
@@ -3083,7 +3102,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
@@ -3120,7 +3141,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
@@ -3157,7 +3180,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L14" s="1"/>
+      <c r="L14" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
@@ -3194,7 +3219,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L15" s="1"/>
+      <c r="L15" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
@@ -3231,7 +3258,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L16" s="1"/>
+      <c r="L16" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
@@ -3268,7 +3297,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L17" s="1"/>
+      <c r="L17" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
@@ -3305,7 +3336,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
@@ -3342,7 +3375,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
@@ -3379,7 +3414,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
@@ -3416,7 +3453,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L21" s="1"/>
+      <c r="L21" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
@@ -3453,7 +3492,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
@@ -3490,7 +3531,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L23" s="1"/>
+      <c r="L23" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
@@ -3527,7 +3570,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
@@ -3564,7 +3609,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L25" s="1"/>
+      <c r="L25" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
@@ -3601,7 +3648,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
@@ -3638,7 +3687,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L27" s="1"/>
+      <c r="L27" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
@@ -3675,7 +3726,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L28" s="1"/>
+      <c r="L28" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
@@ -3712,7 +3765,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L29" s="1"/>
+      <c r="L29" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
@@ -3749,7 +3804,9 @@
         <f t="shared" si="0"/>
         <v>Jan</v>
       </c>
-      <c r="L30" s="1"/>
+      <c r="L30" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
@@ -3786,7 +3843,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L31" s="1"/>
+      <c r="L31" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
@@ -3823,7 +3882,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L32" s="1"/>
+      <c r="L32" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
@@ -3860,7 +3921,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L33" s="1"/>
+      <c r="L33" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
@@ -3897,7 +3960,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L34" s="1"/>
+      <c r="L34" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
@@ -3934,7 +3999,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L35" s="1"/>
+      <c r="L35" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
@@ -3971,7 +4038,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L36" s="1"/>
+      <c r="L36" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
@@ -4008,7 +4077,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L37" s="1"/>
+      <c r="L37" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
@@ -4045,7 +4116,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L38" s="1"/>
+      <c r="L38" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
@@ -4082,7 +4155,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L39" s="1"/>
+      <c r="L39" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
@@ -4119,7 +4194,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L40" s="1"/>
+      <c r="L40" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
@@ -4156,7 +4233,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L41" s="1"/>
+      <c r="L41" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
@@ -4193,7 +4272,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L42" s="1"/>
+      <c r="L42" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
@@ -4230,7 +4311,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L43" s="1"/>
+      <c r="L43" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
@@ -4267,7 +4350,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L44" s="1"/>
+      <c r="L44" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
@@ -4304,7 +4389,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L45" s="1"/>
+      <c r="L45" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
@@ -4341,7 +4428,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L46" s="1"/>
+      <c r="L46" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
@@ -4378,7 +4467,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L47" s="1"/>
+      <c r="L47" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
@@ -4415,7 +4506,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L48" s="1"/>
+      <c r="L48" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
@@ -4452,7 +4545,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L49" s="1"/>
+      <c r="L49" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
@@ -4489,7 +4584,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L50" s="1"/>
+      <c r="L50" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
@@ -4526,7 +4623,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L51" s="1"/>
+      <c r="L51" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
@@ -4563,7 +4662,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L52" s="1"/>
+      <c r="L52" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
@@ -4600,7 +4701,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L53" s="1"/>
+      <c r="L53" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
@@ -4637,7 +4740,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L54" s="1"/>
+      <c r="L54" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
@@ -4674,7 +4779,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L55" s="1"/>
+      <c r="L55" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
@@ -4711,7 +4818,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L56" s="1"/>
+      <c r="L56" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
@@ -4748,7 +4857,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L57" s="1"/>
+      <c r="L57" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
@@ -4785,7 +4896,9 @@
         <f t="shared" si="0"/>
         <v>Feb</v>
       </c>
-      <c r="L58" s="1"/>
+      <c r="L58" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
@@ -4822,7 +4935,9 @@
         <f t="shared" si="0"/>
         <v>Mar</v>
       </c>
-      <c r="L59" s="1"/>
+      <c r="L59" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
@@ -4859,7 +4974,9 @@
         <f t="shared" si="0"/>
         <v>Mar</v>
       </c>
-      <c r="L60" s="1"/>
+      <c r="L60" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
@@ -4896,7 +5013,9 @@
         <f t="shared" si="0"/>
         <v>Mar</v>
       </c>
-      <c r="L61" s="1"/>
+      <c r="L61" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
@@ -4933,7 +5052,9 @@
         <f t="shared" si="0"/>
         <v>Mar</v>
       </c>
-      <c r="L62" s="1"/>
+      <c r="L62" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
@@ -4970,7 +5091,9 @@
         <f t="shared" si="0"/>
         <v>Mar</v>
       </c>
-      <c r="L63" s="1"/>
+      <c r="L63" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
@@ -5007,7 +5130,9 @@
         <f t="shared" si="0"/>
         <v>Mar</v>
       </c>
-      <c r="L64" s="1"/>
+      <c r="L64" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
@@ -5044,7 +5169,9 @@
         <f t="shared" si="0"/>
         <v>Mar</v>
       </c>
-      <c r="L65" s="1"/>
+      <c r="L65" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
@@ -5081,7 +5208,9 @@
         <f t="shared" si="0"/>
         <v>Mar</v>
       </c>
-      <c r="L66" s="1"/>
+      <c r="L66" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
@@ -5118,7 +5247,9 @@
         <f t="shared" si="0"/>
         <v>Mar</v>
       </c>
-      <c r="L67" s="1"/>
+      <c r="L67" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
@@ -5155,7 +5286,9 @@
         <f t="shared" ref="K68:K131" si="1">TEXT(DATE(1976,1,J68),"mmm")</f>
         <v>Mar</v>
       </c>
-      <c r="L68" s="1"/>
+      <c r="L68" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
@@ -5192,7 +5325,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L69" s="1"/>
+      <c r="L69" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
@@ -5229,7 +5364,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L70" s="1"/>
+      <c r="L70" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
@@ -5266,7 +5403,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L71" s="1"/>
+      <c r="L71" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A72" t="s">
@@ -5303,7 +5442,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L72" s="1"/>
+      <c r="L72" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
@@ -5340,7 +5481,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L73" s="1"/>
+      <c r="L73" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
@@ -5377,7 +5520,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L74" s="1"/>
+      <c r="L74" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
@@ -5414,7 +5559,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L75" s="1"/>
+      <c r="L75" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
@@ -5451,7 +5598,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L76" s="1"/>
+      <c r="L76" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
@@ -5488,7 +5637,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L77" s="1"/>
+      <c r="L77" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
@@ -5525,7 +5676,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L78" s="1"/>
+      <c r="L78" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
@@ -5562,7 +5715,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L79" s="1"/>
+      <c r="L79" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A80" t="s">
@@ -5599,7 +5754,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L80" s="1"/>
+      <c r="L80" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
@@ -5636,7 +5793,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L81" s="1"/>
+      <c r="L81" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
@@ -5673,7 +5832,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L82" s="1"/>
+      <c r="L82" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A83" t="s">
@@ -5710,7 +5871,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L83" s="1"/>
+      <c r="L83" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A84" t="s">
@@ -5747,7 +5910,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L84" s="1"/>
+      <c r="L84" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A85" t="s">
@@ -5784,7 +5949,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L85" s="1"/>
+      <c r="L85" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A86" t="s">
@@ -5821,7 +5988,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L86" s="1"/>
+      <c r="L86" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A87" t="s">
@@ -5858,7 +6027,9 @@
         <f t="shared" si="1"/>
         <v>Mar</v>
       </c>
-      <c r="L87" s="1"/>
+      <c r="L87" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A88" t="s">
@@ -5895,7 +6066,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L88" s="1"/>
+      <c r="L88" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
@@ -5932,7 +6105,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L89" s="1"/>
+      <c r="L89" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A90" t="s">
@@ -5969,7 +6144,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L90" s="1"/>
+      <c r="L90" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A91" t="s">
@@ -6006,7 +6183,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L91" s="1"/>
+      <c r="L91" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A92" t="s">
@@ -6043,7 +6222,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L92" s="1"/>
+      <c r="L92" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A93" t="s">
@@ -6080,7 +6261,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L93" s="1"/>
+      <c r="L93" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A94" t="s">
@@ -6117,7 +6300,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L94" s="1"/>
+      <c r="L94" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A95" t="s">
@@ -6154,7 +6339,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L95" s="1"/>
+      <c r="L95" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A96" t="s">
@@ -6191,7 +6378,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L96" s="1"/>
+      <c r="L96" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A97" t="s">
@@ -6228,7 +6417,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L97" s="1"/>
+      <c r="L97" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A98" t="s">
@@ -6265,7 +6456,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L98" s="1"/>
+      <c r="L98" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A99" t="s">
@@ -6302,7 +6495,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L99" s="1"/>
+      <c r="L99" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A100" t="s">
@@ -6339,7 +6534,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L100" s="1"/>
+      <c r="L100" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A101" t="s">
@@ -6376,7 +6573,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L101" s="1"/>
+      <c r="L101" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A102" t="s">
@@ -6413,7 +6612,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L102" s="1"/>
+      <c r="L102" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A103" t="s">
@@ -6450,7 +6651,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L103" s="1"/>
+      <c r="L103" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A104" t="s">
@@ -6487,7 +6690,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L104" s="1"/>
+      <c r="L104" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A105" t="s">
@@ -6524,7 +6729,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L105" s="1"/>
+      <c r="L105" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A106" t="s">
@@ -6561,7 +6768,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L106" s="1"/>
+      <c r="L106" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A107" t="s">
@@ -6598,7 +6807,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L107" s="1"/>
+      <c r="L107" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A108" t="s">
@@ -6635,7 +6846,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L108" s="1"/>
+      <c r="L108" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A109" t="s">
@@ -6672,7 +6885,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L109" s="1"/>
+      <c r="L109" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A110" t="s">
@@ -6709,7 +6924,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L110" s="1"/>
+      <c r="L110" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A111" t="s">
@@ -6746,7 +6963,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L111" s="1"/>
+      <c r="L111" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A112" t="s">
@@ -6783,7 +7002,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L112" s="1"/>
+      <c r="L112" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A113" t="s">
@@ -6820,7 +7041,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L113" s="1"/>
+      <c r="L113" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A114" t="s">
@@ -6857,7 +7080,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L114" s="1"/>
+      <c r="L114" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A115" t="s">
@@ -6894,7 +7119,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L115" s="1"/>
+      <c r="L115" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A116" t="s">
@@ -6931,7 +7158,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L116" s="1"/>
+      <c r="L116" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A117" t="s">
@@ -6968,7 +7197,9 @@
         <f t="shared" si="1"/>
         <v>Apr</v>
       </c>
-      <c r="L117" s="1"/>
+      <c r="L117" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A118" t="s">
@@ -7005,7 +7236,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L118" s="1"/>
+      <c r="L118" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A119" t="s">
@@ -7042,7 +7275,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L119" s="1"/>
+      <c r="L119" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A120" t="s">
@@ -7079,7 +7314,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L120" s="1"/>
+      <c r="L120" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A121" t="s">
@@ -7116,7 +7353,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L121" s="1"/>
+      <c r="L121" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A122" t="s">
@@ -7153,7 +7392,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L122" s="1"/>
+      <c r="L122" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A123" t="s">
@@ -7190,7 +7431,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L123" s="1"/>
+      <c r="L123" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A124" t="s">
@@ -7227,7 +7470,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L124" s="1"/>
+      <c r="L124" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A125" t="s">
@@ -7264,7 +7509,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L125" s="1"/>
+      <c r="L125" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A126" t="s">
@@ -7301,7 +7548,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L126" s="1"/>
+      <c r="L126" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A127" t="s">
@@ -7338,7 +7587,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L127" s="1"/>
+      <c r="L127" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A128" t="s">
@@ -7375,7 +7626,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L128" s="1"/>
+      <c r="L128" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A129" t="s">
@@ -7412,7 +7665,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L129" s="1"/>
+      <c r="L129" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A130" t="s">
@@ -7449,7 +7704,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L130" s="1"/>
+      <c r="L130" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A131" t="s">
@@ -7486,7 +7743,9 @@
         <f t="shared" si="1"/>
         <v>May</v>
       </c>
-      <c r="L131" s="1"/>
+      <c r="L131" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A132" t="s">
@@ -7523,7 +7782,9 @@
         <f t="shared" ref="K132:K195" si="2">TEXT(DATE(1976,1,J132),"mmm")</f>
         <v>May</v>
       </c>
-      <c r="L132" s="1"/>
+      <c r="L132" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A133" t="s">
@@ -7560,7 +7821,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L133" s="1"/>
+      <c r="L133" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A134" t="s">
@@ -7597,7 +7860,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L134" s="1"/>
+      <c r="L134" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A135" t="s">
@@ -7634,7 +7899,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L135" s="1"/>
+      <c r="L135" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A136" t="s">
@@ -7671,7 +7938,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L136" s="1"/>
+      <c r="L136" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A137" t="s">
@@ -7708,7 +7977,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L137" s="1"/>
+      <c r="L137" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A138" t="s">
@@ -7745,7 +8016,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L138" s="1"/>
+      <c r="L138" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A139" t="s">
@@ -7782,7 +8055,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L139" s="1"/>
+      <c r="L139" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A140" t="s">
@@ -7819,7 +8094,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L140" s="1"/>
+      <c r="L140" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A141" t="s">
@@ -7856,7 +8133,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L141" s="1"/>
+      <c r="L141" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A142" t="s">
@@ -7893,7 +8172,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L142" s="1"/>
+      <c r="L142" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A143" t="s">
@@ -7930,7 +8211,9 @@
         <f t="shared" si="2"/>
         <v>May</v>
       </c>
-      <c r="L143" s="1"/>
+      <c r="L143" s="1" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A144" t="s">
@@ -7967,7 +8250,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L144" s="1"/>
+      <c r="L144" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A145" t="s">
@@ -8004,7 +8289,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L145" s="1"/>
+      <c r="L145" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A146" t="s">
@@ -8041,7 +8328,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L146" s="1"/>
+      <c r="L146" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A147" t="s">
@@ -8078,7 +8367,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L147" s="1"/>
+      <c r="L147" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A148" t="s">
@@ -8115,7 +8406,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L148" s="1"/>
+      <c r="L148" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A149" t="s">
@@ -8152,7 +8445,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L149" s="1"/>
+      <c r="L149" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A150" t="s">
@@ -8189,7 +8484,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L150" s="1"/>
+      <c r="L150" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A151" t="s">
@@ -8226,7 +8523,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L151" s="1"/>
+      <c r="L151" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A152" t="s">
@@ -8263,7 +8562,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L152" s="1"/>
+      <c r="L152" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A153" t="s">
@@ -8300,7 +8601,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L153" s="1"/>
+      <c r="L153" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A154" t="s">
@@ -8337,7 +8640,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L154" s="1"/>
+      <c r="L154" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A155" t="s">
@@ -8374,7 +8679,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L155" s="1"/>
+      <c r="L155" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A156" t="s">
@@ -8411,7 +8718,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L156" s="1"/>
+      <c r="L156" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A157" t="s">
@@ -8448,7 +8757,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L157" s="1"/>
+      <c r="L157" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A158" t="s">
@@ -8485,7 +8796,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L158" s="1"/>
+      <c r="L158" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A159" t="s">
@@ -8522,7 +8835,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L159" s="1"/>
+      <c r="L159" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A160" t="s">
@@ -8559,7 +8874,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L160" s="1"/>
+      <c r="L160" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A161" t="s">
@@ -8596,7 +8913,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L161" s="1"/>
+      <c r="L161" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A162" t="s">
@@ -8633,7 +8952,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L162" s="1"/>
+      <c r="L162" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A163" t="s">
@@ -8670,7 +8991,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L163" s="1"/>
+      <c r="L163" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A164" t="s">
@@ -8707,7 +9030,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L164" s="1"/>
+      <c r="L164" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A165" t="s">
@@ -8744,7 +9069,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L165" s="1"/>
+      <c r="L165" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A166" t="s">
@@ -8781,7 +9108,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L166" s="1"/>
+      <c r="L166" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A167" t="s">
@@ -8818,7 +9147,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L167" s="1"/>
+      <c r="L167" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A168" t="s">
@@ -8855,7 +9186,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L168" s="1"/>
+      <c r="L168" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A169" t="s">
@@ -8892,7 +9225,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L169" s="1"/>
+      <c r="L169" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A170" t="s">
@@ -8929,7 +9264,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L170" s="1"/>
+      <c r="L170" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A171" t="s">
@@ -8966,7 +9303,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L171" s="1"/>
+      <c r="L171" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A172" t="s">
@@ -9003,7 +9342,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L172" s="1"/>
+      <c r="L172" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A173" t="s">
@@ -9040,7 +9381,9 @@
         <f t="shared" si="2"/>
         <v>Jun</v>
       </c>
-      <c r="L173" s="1"/>
+      <c r="L173" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A174" t="s">
@@ -9077,7 +9420,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L174" s="1"/>
+      <c r="L174" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A175" t="s">
@@ -9114,7 +9459,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L175" s="1"/>
+      <c r="L175" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A176" t="s">
@@ -9151,7 +9498,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L176" s="1"/>
+      <c r="L176" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A177" t="s">
@@ -9188,7 +9537,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L177" s="1"/>
+      <c r="L177" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A178" t="s">
@@ -9225,7 +9576,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L178" s="1"/>
+      <c r="L178" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A179" t="s">
@@ -9262,7 +9615,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L179" s="1"/>
+      <c r="L179" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A180" t="s">
@@ -9299,7 +9654,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L180" s="1"/>
+      <c r="L180" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A181" t="s">
@@ -9336,7 +9693,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L181" s="1"/>
+      <c r="L181" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A182" t="s">
@@ -9373,7 +9732,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L182" s="1"/>
+      <c r="L182" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A183" t="s">
@@ -9410,7 +9771,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L183" s="1"/>
+      <c r="L183" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A184" t="s">
@@ -9447,7 +9810,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L184" s="1"/>
+      <c r="L184" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A185" t="s">
@@ -9484,7 +9849,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L185" s="1"/>
+      <c r="L185" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A186" t="s">
@@ -9521,7 +9888,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L186" s="1"/>
+      <c r="L186" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A187" t="s">
@@ -9558,7 +9927,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L187" s="1"/>
+      <c r="L187" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A188" t="s">
@@ -9595,7 +9966,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L188" s="1"/>
+      <c r="L188" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A189" t="s">
@@ -9632,7 +10005,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L189" s="1"/>
+      <c r="L189" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A190" t="s">
@@ -9669,7 +10044,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L190" s="1"/>
+      <c r="L190" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A191" t="s">
@@ -9706,7 +10083,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L191" s="1"/>
+      <c r="L191" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A192" t="s">
@@ -9743,7 +10122,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L192" s="1"/>
+      <c r="L192" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A193" t="s">
@@ -9780,7 +10161,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L193" s="1"/>
+      <c r="L193" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A194" t="s">
@@ -9817,7 +10200,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L194" s="1"/>
+      <c r="L194" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A195" t="s">
@@ -9854,7 +10239,9 @@
         <f t="shared" si="2"/>
         <v>Jul</v>
       </c>
-      <c r="L195" s="1"/>
+      <c r="L195" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A196" t="s">
@@ -9891,7 +10278,9 @@
         <f t="shared" ref="K196:K259" si="3">TEXT(DATE(1976,1,J196),"mmm")</f>
         <v>Jul</v>
       </c>
-      <c r="L196" s="1"/>
+      <c r="L196" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A197" t="s">
@@ -9928,7 +10317,9 @@
         <f t="shared" si="3"/>
         <v>Jul</v>
       </c>
-      <c r="L197" s="1"/>
+      <c r="L197" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A198" t="s">
@@ -9965,7 +10356,9 @@
         <f t="shared" si="3"/>
         <v>Jul</v>
       </c>
-      <c r="L198" s="1"/>
+      <c r="L198" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A199" t="s">
@@ -10002,7 +10395,9 @@
         <f t="shared" si="3"/>
         <v>Jul</v>
       </c>
-      <c r="L199" s="1"/>
+      <c r="L199" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A200" t="s">
@@ -10039,7 +10434,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L200" s="1"/>
+      <c r="L200" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A201" t="s">
@@ -10076,7 +10473,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L201" s="1"/>
+      <c r="L201" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A202" t="s">
@@ -10113,7 +10512,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L202" s="1"/>
+      <c r="L202" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A203" t="s">
@@ -10150,7 +10551,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L203" s="1"/>
+      <c r="L203" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A204" t="s">
@@ -10187,7 +10590,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L204" s="1"/>
+      <c r="L204" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A205" t="s">
@@ -10224,7 +10629,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L205" s="1"/>
+      <c r="L205" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A206" t="s">
@@ -10261,7 +10668,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L206" s="1"/>
+      <c r="L206" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A207" t="s">
@@ -10298,7 +10707,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L207" s="1"/>
+      <c r="L207" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A208" t="s">
@@ -10335,7 +10746,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L208" s="1"/>
+      <c r="L208" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A209" t="s">
@@ -10372,7 +10785,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L209" s="1"/>
+      <c r="L209" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A210" t="s">
@@ -10409,7 +10824,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L210" s="1"/>
+      <c r="L210" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A211" t="s">
@@ -10446,7 +10863,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L211" s="1"/>
+      <c r="L211" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A212" t="s">
@@ -10483,7 +10902,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L212" s="1"/>
+      <c r="L212" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A213" t="s">
@@ -10520,7 +10941,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L213" s="1"/>
+      <c r="L213" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A214" t="s">
@@ -10557,7 +10980,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L214" s="1"/>
+      <c r="L214" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A215" t="s">
@@ -10594,7 +11019,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L215" s="1"/>
+      <c r="L215" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A216" t="s">
@@ -10631,7 +11058,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L216" s="1"/>
+      <c r="L216" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A217" t="s">
@@ -10668,7 +11097,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L217" s="1"/>
+      <c r="L217" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A218" t="s">
@@ -10705,7 +11136,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L218" s="1"/>
+      <c r="L218" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A219" t="s">
@@ -10742,7 +11175,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L219" s="1"/>
+      <c r="L219" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A220" t="s">
@@ -10779,7 +11214,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L220" s="1"/>
+      <c r="L220" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A221" t="s">
@@ -10816,7 +11253,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L221" s="1"/>
+      <c r="L221" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A222" t="s">
@@ -10853,7 +11292,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L222" s="1"/>
+      <c r="L222" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A223" t="s">
@@ -10890,7 +11331,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L223" s="1"/>
+      <c r="L223" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A224" t="s">
@@ -10927,7 +11370,9 @@
         <f t="shared" si="3"/>
         <v>Aug</v>
       </c>
-      <c r="L224" s="1"/>
+      <c r="L224" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A225" t="s">
@@ -10964,7 +11409,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L225" s="1"/>
+      <c r="L225" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A226" t="s">
@@ -11001,7 +11448,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L226" s="1"/>
+      <c r="L226" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A227" t="s">
@@ -11038,7 +11487,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L227" s="1"/>
+      <c r="L227" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A228" t="s">
@@ -11075,7 +11526,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L228" s="1"/>
+      <c r="L228" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A229" t="s">
@@ -11112,7 +11565,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L229" s="1"/>
+      <c r="L229" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A230" t="s">
@@ -11149,7 +11604,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L230" s="1"/>
+      <c r="L230" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A231" t="s">
@@ -11186,7 +11643,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L231" s="1"/>
+      <c r="L231" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A232" t="s">
@@ -11223,7 +11682,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L232" s="1"/>
+      <c r="L232" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A233" t="s">
@@ -11260,7 +11721,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L233" s="1"/>
+      <c r="L233" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A234" t="s">
@@ -11297,7 +11760,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L234" s="1"/>
+      <c r="L234" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A235" t="s">
@@ -11334,7 +11799,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L235" s="1"/>
+      <c r="L235" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A236" t="s">
@@ -11371,7 +11838,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L236" s="1"/>
+      <c r="L236" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A237" t="s">
@@ -11408,7 +11877,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L237" s="1"/>
+      <c r="L237" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A238" t="s">
@@ -11445,7 +11916,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L238" s="1"/>
+      <c r="L238" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A239" t="s">
@@ -11482,7 +11955,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L239" s="1"/>
+      <c r="L239" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A240" t="s">
@@ -11519,7 +11994,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L240" s="1"/>
+      <c r="L240" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A241" t="s">
@@ -11556,7 +12033,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L241" s="1"/>
+      <c r="L241" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A242" t="s">
@@ -11593,7 +12072,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L242" s="1"/>
+      <c r="L242" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A243" t="s">
@@ -11630,7 +12111,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L243" s="1"/>
+      <c r="L243" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A244" t="s">
@@ -11667,7 +12150,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L244" s="1"/>
+      <c r="L244" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A245" t="s">
@@ -11704,7 +12189,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L245" s="1"/>
+      <c r="L245" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A246" t="s">
@@ -11741,7 +12228,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L246" s="1"/>
+      <c r="L246" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A247" t="s">
@@ -11778,7 +12267,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L247" s="1"/>
+      <c r="L247" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A248" t="s">
@@ -11815,7 +12306,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L248" s="1"/>
+      <c r="L248" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A249" t="s">
@@ -11852,7 +12345,9 @@
         <f t="shared" si="3"/>
         <v>Sep</v>
       </c>
-      <c r="L249" s="1"/>
+      <c r="L249" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A250" t="s">
@@ -11889,7 +12384,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L250" s="1"/>
+      <c r="L250" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A251" t="s">
@@ -11926,7 +12423,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L251" s="1"/>
+      <c r="L251" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A252" t="s">
@@ -11963,7 +12462,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L252" s="1"/>
+      <c r="L252" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A253" t="s">
@@ -12000,7 +12501,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L253" s="1"/>
+      <c r="L253" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A254" t="s">
@@ -12037,7 +12540,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L254" s="1"/>
+      <c r="L254" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A255" t="s">
@@ -12074,7 +12579,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L255" s="1"/>
+      <c r="L255" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A256" t="s">
@@ -12111,7 +12618,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L256" s="1"/>
+      <c r="L256" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A257" t="s">
@@ -12148,7 +12657,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L257" s="1"/>
+      <c r="L257" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A258" t="s">
@@ -12185,7 +12696,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L258" s="1"/>
+      <c r="L258" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A259" t="s">
@@ -12222,7 +12735,9 @@
         <f t="shared" si="3"/>
         <v>Oct</v>
       </c>
-      <c r="L259" s="1"/>
+      <c r="L259" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A260" t="s">
@@ -12259,7 +12774,9 @@
         <f t="shared" ref="K260:K323" si="4">TEXT(DATE(1976,1,J260),"mmm")</f>
         <v>Oct</v>
       </c>
-      <c r="L260" s="1"/>
+      <c r="L260" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A261" t="s">
@@ -12296,7 +12813,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L261" s="1"/>
+      <c r="L261" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A262" t="s">
@@ -12333,7 +12852,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L262" s="1"/>
+      <c r="L262" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A263" t="s">
@@ -12370,7 +12891,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L263" s="1"/>
+      <c r="L263" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A264" t="s">
@@ -12407,7 +12930,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L264" s="1"/>
+      <c r="L264" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A265" t="s">
@@ -12444,7 +12969,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L265" s="1"/>
+      <c r="L265" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A266" t="s">
@@ -12481,7 +13008,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L266" s="1"/>
+      <c r="L266" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A267" t="s">
@@ -12518,7 +13047,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L267" s="1"/>
+      <c r="L267" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A268" t="s">
@@ -12555,7 +13086,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L268" s="1"/>
+      <c r="L268" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A269" t="s">
@@ -12592,7 +13125,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L269" s="1"/>
+      <c r="L269" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A270" t="s">
@@ -12629,7 +13164,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L270" s="1"/>
+      <c r="L270" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A271" t="s">
@@ -12666,7 +13203,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L271" s="1"/>
+      <c r="L271" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A272" t="s">
@@ -12703,7 +13242,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L272" s="1"/>
+      <c r="L272" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A273" t="s">
@@ -12740,7 +13281,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L273" s="1"/>
+      <c r="L273" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A274" t="s">
@@ -12777,7 +13320,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L274" s="1"/>
+      <c r="L274" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A275" t="s">
@@ -12814,7 +13359,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L275" s="1"/>
+      <c r="L275" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A276" t="s">
@@ -12851,7 +13398,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L276" s="1"/>
+      <c r="L276" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A277" t="s">
@@ -12888,7 +13437,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L277" s="1"/>
+      <c r="L277" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A278" t="s">
@@ -12925,7 +13476,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L278" s="1"/>
+      <c r="L278" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A279" t="s">
@@ -12962,7 +13515,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L279" s="1"/>
+      <c r="L279" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A280" t="s">
@@ -12999,7 +13554,9 @@
         <f t="shared" si="4"/>
         <v>Oct</v>
       </c>
-      <c r="L280" s="1"/>
+      <c r="L280" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A281" t="s">
@@ -13036,7 +13593,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L281" s="1"/>
+      <c r="L281" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A282" t="s">
@@ -13073,7 +13632,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L282" s="1"/>
+      <c r="L282" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A283" t="s">
@@ -13110,7 +13671,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L283" s="1"/>
+      <c r="L283" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A284" t="s">
@@ -13147,7 +13710,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L284" s="1"/>
+      <c r="L284" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A285" t="s">
@@ -13184,7 +13749,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L285" s="1"/>
+      <c r="L285" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A286" t="s">
@@ -13221,7 +13788,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L286" s="1"/>
+      <c r="L286" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A287" t="s">
@@ -13258,7 +13827,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L287" s="1"/>
+      <c r="L287" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A288" t="s">
@@ -13295,7 +13866,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L288" s="1"/>
+      <c r="L288" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A289" t="s">
@@ -13332,7 +13905,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L289" s="1"/>
+      <c r="L289" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A290" t="s">
@@ -13369,7 +13944,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L290" s="1"/>
+      <c r="L290" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A291" t="s">
@@ -13406,7 +13983,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L291" s="1"/>
+      <c r="L291" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A292" t="s">
@@ -13443,7 +14022,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L292" s="1"/>
+      <c r="L292" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A293" t="s">
@@ -13480,7 +14061,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L293" s="1"/>
+      <c r="L293" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A294" t="s">
@@ -13517,7 +14100,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L294" s="1"/>
+      <c r="L294" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A295" t="s">
@@ -13554,7 +14139,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L295" s="1"/>
+      <c r="L295" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A296" t="s">
@@ -13591,7 +14178,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L296" s="1"/>
+      <c r="L296" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A297" t="s">
@@ -13628,7 +14217,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L297" s="1"/>
+      <c r="L297" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A298" t="s">
@@ -13665,7 +14256,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L298" s="1"/>
+      <c r="L298" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A299" t="s">
@@ -13702,7 +14295,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L299" s="1"/>
+      <c r="L299" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A300" t="s">
@@ -13739,7 +14334,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L300" s="1"/>
+      <c r="L300" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A301" t="s">
@@ -13776,7 +14373,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L301" s="1"/>
+      <c r="L301" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A302" t="s">
@@ -13813,7 +14412,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L302" s="1"/>
+      <c r="L302" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="303" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A303" t="s">
@@ -13850,7 +14451,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L303" s="1"/>
+      <c r="L303" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="304" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A304" t="s">
@@ -13887,7 +14490,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L304" s="1"/>
+      <c r="L304" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="305" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A305" t="s">
@@ -13924,7 +14529,9 @@
         <f t="shared" si="4"/>
         <v>Nov</v>
       </c>
-      <c r="L305" s="1"/>
+      <c r="L305" s="1" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A306" t="s">
@@ -13961,7 +14568,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L306" s="1"/>
+      <c r="L306" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A307" t="s">
@@ -13998,7 +14607,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L307" s="1"/>
+      <c r="L307" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A308" t="s">
@@ -14035,7 +14646,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L308" s="1"/>
+      <c r="L308" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="309" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A309" t="s">
@@ -14072,7 +14685,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L309" s="1"/>
+      <c r="L309" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A310" t="s">
@@ -14109,7 +14724,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L310" s="1"/>
+      <c r="L310" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A311" t="s">
@@ -14146,7 +14763,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L311" s="1"/>
+      <c r="L311" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A312" t="s">
@@ -14183,7 +14802,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L312" s="1"/>
+      <c r="L312" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="313" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A313" t="s">
@@ -14220,7 +14841,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L313" s="1"/>
+      <c r="L313" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A314" t="s">
@@ -14257,7 +14880,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L314" s="1"/>
+      <c r="L314" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="315" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A315" t="s">
@@ -14294,7 +14919,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L315" s="1"/>
+      <c r="L315" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="316" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A316" t="s">
@@ -14331,7 +14958,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L316" s="1"/>
+      <c r="L316" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="317" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A317" t="s">
@@ -14368,7 +14997,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L317" s="1"/>
+      <c r="L317" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A318" t="s">
@@ -14405,7 +15036,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L318" s="1"/>
+      <c r="L318" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="319" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A319" t="s">
@@ -14442,7 +15075,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L319" s="1"/>
+      <c r="L319" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A320" t="s">
@@ -14479,7 +15114,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L320" s="1"/>
+      <c r="L320" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="321" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A321" t="s">
@@ -14516,7 +15153,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L321" s="1"/>
+      <c r="L321" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="322" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A322" t="s">
@@ -14553,7 +15192,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L322" s="1"/>
+      <c r="L322" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A323" t="s">
@@ -14590,7 +15231,9 @@
         <f t="shared" si="4"/>
         <v>Dec</v>
       </c>
-      <c r="L323" s="1"/>
+      <c r="L323" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A324" t="s">
@@ -14627,7 +15270,9 @@
         <f t="shared" ref="K324:K333" si="5">TEXT(DATE(1976,1,J324),"mmm")</f>
         <v>Dec</v>
       </c>
-      <c r="L324" s="1"/>
+      <c r="L324" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A325" t="s">
@@ -14664,7 +15309,9 @@
         <f t="shared" si="5"/>
         <v>Dec</v>
       </c>
-      <c r="L325" s="1"/>
+      <c r="L325" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A326" t="s">
@@ -14701,7 +15348,9 @@
         <f t="shared" si="5"/>
         <v>Dec</v>
       </c>
-      <c r="L326" s="1"/>
+      <c r="L326" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="327" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A327" t="s">
@@ -14738,7 +15387,9 @@
         <f t="shared" si="5"/>
         <v>Dec</v>
       </c>
-      <c r="L327" s="1"/>
+      <c r="L327" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A328" t="s">
@@ -14775,7 +15426,9 @@
         <f t="shared" si="5"/>
         <v>Dec</v>
       </c>
-      <c r="L328" s="1"/>
+      <c r="L328" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="329" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A329" t="s">
@@ -14812,7 +15465,9 @@
         <f t="shared" si="5"/>
         <v>Dec</v>
       </c>
-      <c r="L329" s="1"/>
+      <c r="L329" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A330" t="s">
@@ -14849,7 +15504,9 @@
         <f t="shared" si="5"/>
         <v>Dec</v>
       </c>
-      <c r="L330" s="1"/>
+      <c r="L330" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A331" t="s">
@@ -14886,7 +15543,9 @@
         <f t="shared" si="5"/>
         <v>Dec</v>
       </c>
-      <c r="L331" s="1"/>
+      <c r="L331" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A332" t="s">
@@ -14923,7 +15582,9 @@
         <f t="shared" si="5"/>
         <v>Dec</v>
       </c>
-      <c r="L332" s="1"/>
+      <c r="L332" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="333" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A333" t="s">
@@ -14960,7 +15621,9 @@
         <f t="shared" si="5"/>
         <v>Dec</v>
       </c>
-      <c r="L333" s="1"/>
+      <c r="L333" s="1" t="s">
+        <v>742</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>